<commit_message>
fix: survey missing and additional comment
</commit_message>
<xml_diff>
--- a/outputs/survey_additional_comments.xlsx
+++ b/outputs/survey_additional_comments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,18 +453,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Healthsheet</t>
+          <t>Accountability Documentation</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Data generator</t>
+          <t>Both</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">I found the healthsheet very interesting and helpful guiding through the filling process.
-</t>
+          <t>Data privacy is of utmost importance while gathering as much information as can be possible. As per IRB protocol, every subject should go through consent form signatures as well as provide honest feedback and information during the experiment for data collection. Their safe space while following all guidelines and protocols is very important.</t>
         </is>
       </c>
     </row>
@@ -491,6 +490,92 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Dataset Nutrition Label</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Both</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>The dataset nutrition label is comprehensive but could be enhanced by including sections specifically addressing bias detection and mitigation, detailed demographic information, and ethical considerations. These elements are crucial for developing responsible AI/ML models in clinical research.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Dataset Nutrition Label</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Both</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It seems less useful than the data card. </t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Healthsheet</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Data generator</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I found the healthsheet very interesting and helpful guiding through the filling process.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Healthsheet</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Both</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>The healthsheet is comprehensive but could be improved by including sections on bias mitigation, ethical considerations, and data provenance. These additions would enhance the transparency and reliability of the dataset for developing AI/ML models responsibly.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Healthsheet</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Both</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It seems more difficult to collect </t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>